<commit_message>
Do Mann-Whitney U Test (p-value = 0.003)
</commit_message>
<xml_diff>
--- a/results/LIWC-22 Results - female - LIWC Analysis.xlsx
+++ b/results/LIWC-22 Results - female - LIWC Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Projects\second_study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben Levy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53CC9B78-E981-4F27-A0F4-DC0E23E1A9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5AC3EB-A5D1-48E1-90C2-797B8B03C691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIWC-22 Results - female - LIWC" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,26 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'LIWC-22 Results - female - LIWC'!$T$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'LIWC-22 Results - female - LIWC'!$T$2:$T$165</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'LIWC-22 Results - female - LIWC'!$T$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'LIWC-22 Results - female - LIWC'!$T$2:$T$165</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="193">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -590,12 +601,27 @@
   </si>
   <si>
     <t>n=</t>
+  </si>
+  <si>
+    <t>H_0: μ_f=μ_m</t>
+  </si>
+  <si>
+    <t>CDI:</t>
+  </si>
+  <si>
+    <t>H_a: μ_f &lt; μ_m</t>
+  </si>
+  <si>
+    <t>Mann-Whitney U Test (unpaired, two-samples)</t>
+  </si>
+  <si>
+    <t>p-value: 0.002764 &lt; alpha=0.05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2133,14 +2159,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T169"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="R173" sqref="R173"/>
+    <sheetView tabSelected="1" topLeftCell="Q128" workbookViewId="0">
+      <selection activeCell="V139" sqref="V139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="22" max="22" width="45.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -9818,7 +9847,7 @@
         <v>9.8999999999999932</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>9392</v>
       </c>
@@ -9878,7 +9907,7 @@
         <v>-3.3300000000000045</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>9498</v>
       </c>
@@ -9938,7 +9967,7 @@
         <v>5.7599999999999945</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>9551</v>
       </c>
@@ -9998,7 +10027,7 @@
         <v>17.14</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>9591</v>
       </c>
@@ -10058,7 +10087,7 @@
         <v>2.9999999999999805E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>9594</v>
       </c>
@@ -10118,7 +10147,7 @@
         <v>2.089999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>9634</v>
       </c>
@@ -10177,8 +10206,11 @@
         <f t="shared" si="2"/>
         <v>-6.66</v>
       </c>
-    </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V134" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>9635</v>
       </c>
@@ -10237,8 +10269,11 @@
         <f t="shared" si="2"/>
         <v>7.7200000000000042</v>
       </c>
-    </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V135" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>9720</v>
       </c>
@@ -10297,8 +10332,11 @@
         <f t="shared" si="2"/>
         <v>8.3800000000000026</v>
       </c>
-    </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V136" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>9735</v>
       </c>
@@ -10357,8 +10395,11 @@
         <f t="shared" si="2"/>
         <v>0.33000000000000718</v>
       </c>
-    </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V137" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>9750</v>
       </c>
@@ -10417,8 +10458,11 @@
         <f t="shared" si="2"/>
         <v>4.6300000000000026</v>
       </c>
-    </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V138" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>9785</v>
       </c>
@@ -10478,7 +10522,7 @@
         <v>-2.1299999999999968</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>9793</v>
       </c>
@@ -10538,7 +10582,7 @@
         <v>-14.439999999999996</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>9887</v>
       </c>
@@ -10598,7 +10642,7 @@
         <v>-6.8099999999999987</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>9889</v>
       </c>
@@ -10658,7 +10702,7 @@
         <v>12.400000000000009</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>10018</v>
       </c>
@@ -10718,7 +10762,7 @@
         <v>-1.1400000000000055</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>10039</v>
       </c>
@@ -12095,7 +12139,7 @@
         <v>2.5815243902439016</v>
       </c>
       <c r="T167">
-        <f t="shared" ref="S167:T167" si="4">AVERAGE(T2:T165)</f>
+        <f t="shared" ref="T167" si="4">AVERAGE(T2:T165)</f>
         <v>-1.7112804878048788</v>
       </c>
     </row>
@@ -12156,7 +12200,7 @@
         <v>1.2892189077265004</v>
       </c>
       <c r="T168">
-        <f t="shared" ref="S168:T168" si="6">_xlfn.STDEV.S(T2:T165)</f>
+        <f t="shared" ref="T168" si="6">_xlfn.STDEV.S(T2:T165)</f>
         <v>8.351353452301078</v>
       </c>
     </row>

</xml_diff>